<commit_message>
[ASSIGN8] first attempt of parallelization
</commit_message>
<xml_diff>
--- a/assignment_08/data/measurments_ex01.xlsx
+++ b/assignment_08/data/measurments_ex01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidedesclavis/Documents/WS-2020:21/ParalleleSysteme/GIT/parallel_systems/assignment_08/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F4BF645-67D3-1443-8485-7C1290DC8F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADC0E21-9B39-D343-A682-8B49F3D2F872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="900" windowWidth="28040" windowHeight="16620" xr2:uid="{D8267629-24AD-0E4B-8DD7-5997E4880D31}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{D8267629-24AD-0E4B-8DD7-5997E4880D31}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Measurments Matrix Multiplication</t>
   </si>
@@ -63,15 +63,19 @@
     <t>seq local</t>
   </si>
   <si>
-    <t>seq lcc2</t>
+    <t>seq local -O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omp </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -117,12 +121,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -440,31 +444,32 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -493,22 +498,22 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>7.7800000000000005E-4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>6.483E-3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>0.74351400000000001</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>19.029693999999999</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>252.65250499999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>251.87815800000001</v>
       </c>
     </row>
@@ -516,41 +521,57 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="4">
+        <v>1.7200000000000001E-4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.1589999999999999E-3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.26002599999999998</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4.4229019999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>88.539108999999996</v>
+      </c>
+      <c r="G6" s="4">
+        <v>147.00296499999999</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ASSIGN9] Added analysis.txt from gprof
</commit_message>
<xml_diff>
--- a/assignment_08/data/measurments_ex01.xlsx
+++ b/assignment_08/data/measurments_ex01.xlsx
@@ -5,67 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel/Documents/parallel_systems/assignment_08/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidedesclavis/Documents/WS-2020:21/ParalleleSysteme/GIT/parallel_systems/assignment_08/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79D723AE-F093-C64B-B93E-7FC96A2E05BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07270988-FC1D-A045-83F2-549DA8A91E58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28560" windowHeight="16620" xr2:uid="{D8267629-24AD-0E4B-8DD7-5997E4880D31}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28560" windowHeight="16580" xr2:uid="{D8267629-24AD-0E4B-8DD7-5997E4880D31}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$A$29</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$A$30</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Tabelle1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Tabelle1!$B$31:$E$31</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Tabelle1!$B$32:$E$32</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Tabelle1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Tabelle1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Tabelle1!$B$35:$E$35</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Tabelle1!$B$36:$E$36</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Tabelle1!$A$52</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Tabelle1!$A$53</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Tabelle1!$A$54</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$A$31</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Tabelle1!$A$55</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Tabelle1!$A$56</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Tabelle1!$A$57</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Tabelle1!$A$58</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Tabelle1!$B$51:$E$51</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Tabelle1!$B$52:$E$52</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Tabelle1!$B$53:$E$53</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Tabelle1!$B$54:$E$54</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Tabelle1!$B$55:$E$55</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Tabelle1!$B$56:$E$56</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Tabelle1!$A$32</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Tabelle1!$B$57:$E$57</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Tabelle1!$B$58:$E$58</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Tabelle1!$A$29</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Tabelle1!$A$30</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Tabelle1!$A$31</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Tabelle1!$A$32</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Tabelle1!$A$33</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Tabelle1!$A$34</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Tabelle1!$A$35</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Tabelle1!$A$36</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$A$33</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Tabelle1!$B$28:$E$28</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Tabelle1!$B$29:$E$29</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Tabelle1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Tabelle1!$B$31:$E$31</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Tabelle1!$B$32:$E$32</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Tabelle1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Tabelle1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Tabelle1!$B$35:$E$35</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Tabelle1!$B$36:$E$36</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Tabelle1!$A$34</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Tabelle1!$A$35</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Tabelle1!$A$36</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Tabelle1!$B$28:$E$28</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Tabelle1!$B$29:$E$29</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -271,14 +220,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -300,1663 +249,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Walltimes</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>seq </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$5:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.7127600000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>163.26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>532.59</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$6:$E$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.154978</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2607710000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.154431000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35.420654999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.8914999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67009099999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3239640000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.414355</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000015-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$8:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.7340000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.457872</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6376909999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.586509</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000016-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="13"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$9:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.3335E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.38180599999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7500529999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.7681009999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="14"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$10:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.9191999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.30993900000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.335464</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8357559999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000018-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="15"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$11:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.8948999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.233792</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.936304</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.4768039999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000019-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="16"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$12:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.0092000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23519300000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.78793</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.7410410000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001A-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="17"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.6648E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.233291</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.575224</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0068159999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001B-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>seq </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$5:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.7127600000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>163.26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>532.59</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$6:$E$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.154978</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2607710000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.154431000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35.420654999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.8914999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67009099999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3239640000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.414355</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="12"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$8:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.7340000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.457872</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6376909999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.586509</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="13"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="star"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$9:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.3335E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.38180599999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7500529999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.7681009999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="14"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$10:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.9191999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.30993900000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.335464</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8357559999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="15"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="plus"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$11:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.8948999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.233792</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.936304</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.4768039999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="16"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="dot"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$12:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.0092000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23519300000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.78793</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.7410410000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="17"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>optomp8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="dash"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>NxN= 500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>NxN= 1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>NxN= 2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>NxN= 3000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.6648E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.233291</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.575224</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0068159999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-B12E-F34B-957F-DC4A48F8D11B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="878227999"/>
-        <c:axId val="819908991"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="878227999"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Size</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="819908991"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="819908991"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="878227999"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst/>
-  </c:chart>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -3144,7 +1436,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -5117,7 +3409,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -7091,7 +5383,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -8172,7 +6464,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -9130,7 +7422,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -10119,7 +8411,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -11004,6 +9296,1193 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Walltimes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>seq </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.7127600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>532.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.154978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2607710000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.154431000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.420654999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.8914999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67009099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3239640000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.414355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.7340000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.457872</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6376909999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.586509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.3335E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38180599999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7500529999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7681009999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.9191999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30993900000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.335464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8357559999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.8948999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.233792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.936304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4768039999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dot"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0092000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23519300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.78793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7410410000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optomp8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NxN= 500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NxN= 1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NxN= 2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NxN= 3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$13:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.6648E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.233291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.575224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0068159999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-3271-8B46-AC79-16975FDD3ACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="878227999"/>
+        <c:axId val="819908991"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="878227999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="819908991"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="819908991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="878227999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11284,6 +10763,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
@@ -14885,44 +14404,529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B108BFA4-93A2-F042-A9D3-DB05463F129D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
@@ -14955,7 +14959,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14993,7 +14997,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15031,7 +15035,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15067,7 +15071,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15103,7 +15107,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15139,7 +15143,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15168,6 +15172,44 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Diagramm 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3275EE1F-DA94-1D4D-A992-9693D454A5B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -15483,8 +15525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84ACD18E-C002-2848-823A-70F06B249446}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="U24" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15494,16 +15536,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -15687,13 +15729,13 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
@@ -15714,19 +15756,19 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="9">
         <f>B5/B6</f>
         <v>11.051633135025616</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <f t="shared" ref="C18:E18" si="0">C5/C6</f>
         <v>16.25196011012309</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <f t="shared" si="0"/>
         <v>16.077710311882566</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="9">
         <f t="shared" si="0"/>
         <v>15.036142047627298</v>
       </c>
@@ -15735,19 +15777,19 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="9">
         <f>B5/B7</f>
         <v>19.262891525614354</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="9">
         <f t="shared" ref="C19:E19" si="1">C5/C7</f>
         <v>30.577936429529718</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <f t="shared" si="1"/>
         <v>30.665120951231074</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="9">
         <f t="shared" si="1"/>
         <v>28.92254439539153</v>
       </c>
@@ -15756,19 +15798,19 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="9">
         <f>B5/B8</f>
         <v>29.870247645622602</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="9">
         <f t="shared" ref="C20:E20" si="2">C5/C8</f>
         <v>44.750497955760558</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <f t="shared" si="2"/>
         <v>44.880117635060259</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="9">
         <f t="shared" si="2"/>
         <v>42.314354202583104</v>
       </c>
@@ -15777,19 +15819,19 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <f>B5/B9</f>
         <v>32.113246461048092</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <f>C5/C9</f>
         <v>53.66599791517158</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <f t="shared" ref="D21:E21" si="3">D5/D9</f>
         <v>59.366128580067368</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="9">
         <f t="shared" si="3"/>
         <v>54.523392008334071</v>
       </c>
@@ -15798,19 +15840,19 @@
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <f>B5/B10</f>
         <v>43.701775872627074</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <f t="shared" ref="C22:E22" si="4">C5/C10</f>
         <v>66.109782892762766</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <f t="shared" si="4"/>
         <v>69.90473841600641</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="9">
         <f t="shared" si="4"/>
         <v>67.9691914857992</v>
       </c>
@@ -15819,19 +15861,19 @@
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <f>B5/B11</f>
         <v>43.974428098282374</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <f t="shared" ref="C23:E23" si="5">C5/C11</f>
         <v>87.642006569942509</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <f t="shared" si="5"/>
         <v>84.315272808401986</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="9">
         <f t="shared" si="5"/>
         <v>82.230371646262583</v>
       </c>
@@ -15840,19 +15882,19 @@
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <f>B5/B12</f>
         <v>42.720742292726726</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="9">
         <f t="shared" ref="C24:E24" si="6">C5/C12</f>
         <v>87.119939794126509</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <f t="shared" si="6"/>
         <v>91.312299698534048</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="9">
         <f t="shared" si="6"/>
         <v>92.76888982329163</v>
       </c>
@@ -15861,19 +15903,19 @@
       <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="9">
         <f>B5/B13</f>
         <v>46.735428945645054</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <f t="shared" ref="C25:E25" si="7">C5/C13</f>
         <v>87.830220625742086</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <f t="shared" si="7"/>
         <v>103.64240260432801</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="9">
         <f t="shared" si="7"/>
         <v>106.37299233684642</v>
       </c>
@@ -15882,13 +15924,13 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
@@ -16074,13 +16116,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
@@ -16101,19 +16143,19 @@
       <c r="A41" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="8">
         <f>B6/B7</f>
         <v>1.742990496541641</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="8">
         <f t="shared" ref="C41:E41" si="16">C6/C7</f>
         <v>1.8814922152364382</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="8">
         <f t="shared" si="16"/>
         <v>1.9073064731467004</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="8">
         <f t="shared" si="16"/>
         <v>1.9235349269632303</v>
       </c>
@@ -16122,19 +16164,19 @@
       <c r="A42" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="8">
         <f>B6/B8</f>
         <v>2.7027903732124172</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="8">
         <f t="shared" ref="C42:E42" si="17">C6/C8</f>
         <v>2.7535446587692634</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="8">
         <f t="shared" si="17"/>
         <v>2.7914495761184779</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="8">
         <f t="shared" si="17"/>
         <v>2.8141762739771607</v>
       </c>
@@ -16143,19 +16185,19 @@
       <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="8">
         <f>B6/B9</f>
         <v>2.9057466954157682</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="8">
         <f t="shared" ref="C43:E43" si="18">C6/C9</f>
         <v>3.3021246392146799</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="8">
         <f t="shared" si="18"/>
         <v>3.6924492000699627</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="8">
         <f t="shared" si="18"/>
         <v>3.6261556877841454</v>
       </c>
@@ -16164,19 +16206,19 @@
       <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="8">
         <f>B6/B10</f>
         <v>3.9543274137579103</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="8">
         <f t="shared" ref="C44:E44" si="19">C6/C10</f>
         <v>4.0678036645920645</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="8">
         <f t="shared" si="19"/>
         <v>4.3479287199460153</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="8">
         <f t="shared" si="19"/>
         <v>4.5203876945632304</v>
       </c>
@@ -16185,19 +16227,19 @@
       <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="8">
         <f>B6/B11</f>
         <v>3.9789981771033922</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="8">
         <f t="shared" ref="C45:E45" si="20">C6/C11</f>
         <v>5.392703770873255</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="8">
         <f t="shared" si="20"/>
         <v>5.2442338599724012</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="8">
         <f t="shared" si="20"/>
         <v>5.4688477526878998</v>
       </c>
@@ -16206,19 +16248,19 @@
       <c r="A46" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="8">
         <f>B6/B12</f>
         <v>3.8655592138082411</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="8">
         <f t="shared" ref="C46:E46" si="21">C6/C12</f>
         <v>5.36058045945245</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="8">
         <f t="shared" si="21"/>
         <v>5.6794343178983517</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="8">
         <f t="shared" si="21"/>
         <v>6.1697268840267814</v>
       </c>
@@ -16227,31 +16269,31 @@
       <c r="A47" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="8">
         <f>B6/B13</f>
         <v>4.2288255839336388</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="8">
         <f t="shared" ref="C47:D47" si="22">C6/C13</f>
         <v>5.4042847773810392</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="8">
         <f t="shared" si="22"/>
         <v>6.446340964840557</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="8">
         <f>E6/E13</f>
         <v>7.0744870592408429</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>

</xml_diff>